<commit_message>
Lookup and Samples variables changed
</commit_message>
<xml_diff>
--- a/Example 5/output/Result.xlsx
+++ b/Example 5/output/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\Thesis\ColorMatching\Example 5\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47005EC-D96F-4004-BDFB-6DC39EF3AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD272BB4-2E10-477D-86B4-62BE0256E61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="4155" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4800" yWindow="4155" windowWidth="14400" windowHeight="10755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Method name</t>
   </si>
   <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>in-gamut</t>
+  </si>
+  <si>
     <t>Mean RMS</t>
   </si>
   <si>
@@ -64,37 +73,46 @@
     <t>Principal Component Coordinates</t>
   </si>
   <si>
-    <t>0.01088</t>
-  </si>
-  <si>
-    <t>0.62061</t>
-  </si>
-  <si>
-    <t>0.0759</t>
-  </si>
-  <si>
-    <t>0.99973</t>
-  </si>
-  <si>
-    <t>0.00073</t>
-  </si>
-  <si>
-    <t>0.0441</t>
-  </si>
-  <si>
-    <t>0.03936</t>
-  </si>
-  <si>
-    <t>2.59515</t>
-  </si>
-  <si>
-    <t>0.00367</t>
-  </si>
-  <si>
-    <t>0.31721</t>
-  </si>
-  <si>
-    <t>0.9973</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>0.12782</t>
+  </si>
+  <si>
+    <t>7.73038</t>
+  </si>
+  <si>
+    <t>0.11218</t>
+  </si>
+  <si>
+    <t>0.98709</t>
+  </si>
+  <si>
+    <t>0.00173</t>
+  </si>
+  <si>
+    <t>2.13649</t>
+  </si>
+  <si>
+    <t>0.01825</t>
+  </si>
+  <si>
+    <t>86.38423</t>
+  </si>
+  <si>
+    <t>0.00143</t>
+  </si>
+  <si>
+    <t>0.8256</t>
+  </si>
+  <si>
+    <t>0.72739</t>
   </si>
   <si>
     <t>1.0</t>
@@ -103,37 +121,40 @@
     <t>XYZ</t>
   </si>
   <si>
-    <t>0.0102</t>
-  </si>
-  <si>
-    <t>1.05555</t>
-  </si>
-  <si>
-    <t>0.03093</t>
-  </si>
-  <si>
-    <t>0.99993</t>
-  </si>
-  <si>
-    <t>0.00067</t>
-  </si>
-  <si>
-    <t>0.0429</t>
-  </si>
-  <si>
-    <t>0.14141</t>
-  </si>
-  <si>
-    <t>3.89937</t>
-  </si>
-  <si>
-    <t>0.0041</t>
-  </si>
-  <si>
-    <t>0.10908</t>
-  </si>
-  <si>
-    <t>0.99956</t>
+    <t>130</t>
+  </si>
+  <si>
+    <t>0.05388</t>
+  </si>
+  <si>
+    <t>3.4832</t>
+  </si>
+  <si>
+    <t>0.05029</t>
+  </si>
+  <si>
+    <t>0.99908</t>
+  </si>
+  <si>
+    <t>0.00266</t>
+  </si>
+  <si>
+    <t>0.52166</t>
+  </si>
+  <si>
+    <t>0.36752</t>
+  </si>
+  <si>
+    <t>28.32849</t>
+  </si>
+  <si>
+    <t>0.00611</t>
+  </si>
+  <si>
+    <t>0.32387</t>
+  </si>
+  <si>
+    <t>0.98862</t>
   </si>
 </sst>
 </file>
@@ -512,25 +533,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,87 +596,114 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>